<commit_message>
Quick update to power budget
</commit_message>
<xml_diff>
--- a/Hardware/BBB Cape/PowerBudget.xlsx
+++ b/Hardware/BBB Cape/PowerBudget.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Device</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Total Power</t>
   </si>
   <si>
-    <t>Copernicus II</t>
-  </si>
-  <si>
     <t>Max Power Consumed (mA)</t>
   </si>
   <si>
@@ -48,6 +45,15 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>ADAFruit Ultimate GPS</t>
+  </si>
+  <si>
+    <t>M150</t>
   </si>
 </sst>
 </file>
@@ -376,15 +382,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -394,7 +400,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -405,22 +411,22 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B2">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <f>B2*C2</f>
-        <v>44</v>
+        <f>C2*B2</f>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>0.01</v>
@@ -435,33 +441,66 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>5</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <f>B4*C4</f>
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B5">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
       <c r="D5">
-        <f>SUM(D2:D4)</f>
-        <v>84.08</v>
+        <f>C5*B5</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <f>1.8/170</f>
+        <v>1.0588235294117647E-2</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <f>C6*B6</f>
+        <v>5.2941176470588235E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <f>SUM(D2:D6)</f>
+        <v>62.132941176470588</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>